<commit_message>
08.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>RType</t>
   </si>
@@ -132,12 +132,6 @@
     <t>DEL-0179</t>
   </si>
   <si>
-    <t>DSR-0247</t>
-  </si>
-  <si>
-    <t>Naldanga</t>
-  </si>
-  <si>
     <t>Natore</t>
   </si>
   <si>
@@ -147,34 +141,19 @@
     <t>ZSO-0022</t>
   </si>
   <si>
-    <t>Bismillah Mobile Shop</t>
-  </si>
-  <si>
-    <t>Md Shoriful Islam Sumon</t>
-  </si>
-  <si>
-    <t>Mohammod Ali Plaza, Naldanga.</t>
-  </si>
-  <si>
-    <t>Bismillah Electronics 2</t>
-  </si>
-  <si>
-    <t>Singra</t>
-  </si>
-  <si>
-    <t>Md Mizanur Rahman Mintu</t>
-  </si>
-  <si>
-    <t>Upozilla Road, Singra.</t>
-  </si>
-  <si>
-    <t>Liza Telecom</t>
-  </si>
-  <si>
-    <t>Md Liton Pramanik</t>
-  </si>
-  <si>
-    <t>Somospara, Singra.</t>
+    <t>DSR-0248</t>
+  </si>
+  <si>
+    <t>Utsob Telecom</t>
+  </si>
+  <si>
+    <t>Gurudaspur</t>
+  </si>
+  <si>
+    <t>CM Shopping Complex, Chaskoir</t>
+  </si>
+  <si>
+    <t>Md Mithun Ali</t>
   </si>
 </sst>
 </file>
@@ -621,7 +600,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E16" sqref="E14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -715,16 +694,16 @@
         <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
@@ -732,151 +711,83 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1723266045</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="J2" s="5">
-        <v>1303531985</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5">
-        <v>1303531985</v>
+        <v>1723266045</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="T2" s="5">
-        <v>1303531985</v>
+        <v>1723266045</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1">
-      <c r="A3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1732403462</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="5">
-        <v>1732403462</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="5">
-        <v>1732403462</v>
-      </c>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="5">
-        <v>1723568379</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="5">
-        <v>1723568379</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="5">
-        <v>1723568379</v>
-      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="5"/>
@@ -1185,7 +1096,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
06.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="71">
   <si>
     <t>RType</t>
   </si>
@@ -174,13 +174,61 @@
     <t>Jonail Bazar, Baraigram, Natore.</t>
   </si>
   <si>
-    <t>Dolon Mobile</t>
-  </si>
-  <si>
-    <t>Dolon</t>
-  </si>
-  <si>
-    <t>Laxmicole, Baraigram, Natore.</t>
+    <t>Sohan Electric &amp; Hardware</t>
+  </si>
+  <si>
+    <t>Md Sohel Rana</t>
+  </si>
+  <si>
+    <t>Saheb Bazar, Baraigram, Natore.</t>
+  </si>
+  <si>
+    <t>DSR-0619</t>
+  </si>
+  <si>
+    <t>Noor Telecom</t>
+  </si>
+  <si>
+    <t>Md Nozrul Islam</t>
+  </si>
+  <si>
+    <t>Bonpara, Natore.</t>
+  </si>
+  <si>
+    <t>Ma Germents</t>
+  </si>
+  <si>
+    <t>Bagatipara</t>
+  </si>
+  <si>
+    <t>Sabibur &amp; Sajrul</t>
+  </si>
+  <si>
+    <t>Tamaltola,Bagatipara, Natore.</t>
+  </si>
+  <si>
+    <t>DSR-0350</t>
+  </si>
+  <si>
+    <t>SM Enterprise</t>
+  </si>
+  <si>
+    <t>Puthia</t>
+  </si>
+  <si>
+    <t>Md Sofiqul Islam</t>
+  </si>
+  <si>
+    <t>Mollapara Bazar, Puthia, Rajshahi.</t>
+  </si>
+  <si>
+    <t>Rajshahi</t>
+  </si>
+  <si>
+    <t>Ashim Exclusive Showroom</t>
+  </si>
+  <si>
+    <t>Sree Ashim Kumar</t>
   </si>
 </sst>
 </file>
@@ -283,17 +331,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,6 +359,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,325 +683,512 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E16:E18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:20" s="16" customFormat="1" ht="15.75">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:20" s="16" customFormat="1">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="12">
         <v>1733193387</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12">
         <v>1733193387</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="12">
         <v>1733193387</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:20" s="16" customFormat="1">
+      <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="12">
         <v>1717299513</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5">
+      <c r="O3" s="12"/>
+      <c r="P3" s="12">
         <v>1717299513</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="12">
         <v>1717299513</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="12">
+        <v>1739489812</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5" t="s">
+      <c r="O4" s="12"/>
+      <c r="P4" s="12">
+        <v>1739489812</v>
+      </c>
+      <c r="Q4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="5"/>
+      <c r="T4" s="12">
+        <v>1739489812</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="A5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1731003227</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12">
+        <v>1731003227</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="12">
+        <v>1731003227</v>
+      </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1725093894</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12">
+        <v>1725093894</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="12">
+        <v>1725093894</v>
+      </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="15">
+        <v>1751412045</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="15">
+        <v>1751412045</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="15">
+        <v>1751412045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1780996696</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12">
+        <v>1780996696</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="12">
+        <v>1780996696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -963,214 +1209,214 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="6" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="2.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1198,36 +1444,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
15.09.2020 Mc Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>RType</t>
   </si>
@@ -141,46 +141,49 @@
     <t>ZSO-0022</t>
   </si>
   <si>
-    <t>DSR-0248</t>
-  </si>
-  <si>
-    <t>Baraigram</t>
-  </si>
-  <si>
     <t>DSR-0350</t>
   </si>
   <si>
-    <t>Noman Enterprise</t>
-  </si>
-  <si>
     <t>Lalpur</t>
   </si>
   <si>
-    <t>Md  Johurul Islam</t>
-  </si>
-  <si>
     <t>Abdulpur, Lalpur, Natore.</t>
   </si>
   <si>
-    <t>Ma Digital Studio &amp; Electronics</t>
-  </si>
-  <si>
-    <t>Gurudaspur</t>
-  </si>
-  <si>
-    <t>Md Babul Akter(Babu)</t>
-  </si>
-  <si>
-    <t>Edilpur, Gurudaspur, Natore.</t>
-  </si>
-  <si>
-    <t>Dolon Mobile</t>
-  </si>
-  <si>
-    <t>Dolon</t>
-  </si>
-  <si>
-    <t>Laxmicole, Baraigram, Natore.</t>
+    <t>Sinja Telecom</t>
+  </si>
+  <si>
+    <t>Md Sanowar Hosen(Sujon)</t>
+  </si>
+  <si>
+    <t>DSR-0349</t>
+  </si>
+  <si>
+    <t>Anika Telecom</t>
+  </si>
+  <si>
+    <t>Bagha</t>
+  </si>
+  <si>
+    <t>Md Anisur Rahman(Azad)</t>
+  </si>
+  <si>
+    <t>Monigram Bazar, Bagha, Rajshahi.</t>
+  </si>
+  <si>
+    <t>Rajshahi</t>
+  </si>
+  <si>
+    <t>Fatema Telecom 2</t>
+  </si>
+  <si>
+    <t>Md Kutub Uddin</t>
+  </si>
+  <si>
+    <t>Oalia Bazar, Lalpur, Natore.</t>
+  </si>
+  <si>
+    <t>DSR-0619</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I18" sqref="I17:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,16 +736,16 @@
         <v>37</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
@@ -750,26 +753,26 @@
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="12">
-        <v>1718056926</v>
+        <v>1723771230</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>40</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O2" s="12"/>
       <c r="P2" s="12">
-        <v>1718056926</v>
+        <v>1723771230</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>36</v>
@@ -781,7 +784,7 @@
         <v>35</v>
       </c>
       <c r="T2" s="12">
-        <v>1718056926</v>
+        <v>1723771230</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1">
@@ -789,16 +792,16 @@
         <v>37</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
@@ -806,26 +809,26 @@
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J3" s="12">
-        <v>1724426544</v>
+        <v>1748937325</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>40</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="12">
-        <v>1724426544</v>
+        <v>1748937325</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>36</v>
@@ -837,7 +840,7 @@
         <v>35</v>
       </c>
       <c r="T3" s="12">
-        <v>1724426544</v>
+        <v>1748937325</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -845,7 +848,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>52</v>
@@ -865,7 +868,7 @@
         <v>53</v>
       </c>
       <c r="J4" s="12">
-        <v>1710729455</v>
+        <v>1719132820</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>38</v>
@@ -881,7 +884,7 @@
       </c>
       <c r="O4" s="12"/>
       <c r="P4" s="12">
-        <v>1710729455</v>
+        <v>1719132820</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>36</v>
@@ -893,7 +896,7 @@
         <v>35</v>
       </c>
       <c r="T4" s="12">
-        <v>1710729455</v>
+        <v>1719132820</v>
       </c>
     </row>
     <row r="5" spans="1:20">

</xml_diff>

<commit_message>
18.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
   <si>
     <t>RType</t>
   </si>
@@ -97,55 +97,85 @@
     <t>ZSO-0022</t>
   </si>
   <si>
-    <t>Rajshahi</t>
-  </si>
-  <si>
-    <t>Mamun Telecom</t>
-  </si>
-  <si>
-    <t>Puthia</t>
-  </si>
-  <si>
-    <t>Md Mamunur Rashid</t>
-  </si>
-  <si>
-    <t>Masum Electronics</t>
-  </si>
-  <si>
-    <t>Naldanga</t>
-  </si>
-  <si>
-    <t>Md Masum Molla</t>
-  </si>
-  <si>
-    <t>Basudebpur, Naldanga</t>
-  </si>
-  <si>
-    <t>DSR-0351</t>
-  </si>
-  <si>
-    <t>DSR-0247</t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>Moom Telecom</t>
-  </si>
-  <si>
-    <t>Doyarampur</t>
-  </si>
-  <si>
-    <t>Md Mojnu Pramanic</t>
-  </si>
-  <si>
-    <t>M.K Sopping Complex, Doyarampur</t>
+    <t>DSR-0619</t>
+  </si>
+  <si>
+    <t>Sahara Telecom</t>
+  </si>
+  <si>
+    <t>Lalpur</t>
+  </si>
+  <si>
+    <t>Md Shahin Ali</t>
+  </si>
+  <si>
+    <t>Abdulpur, Lalpur, Natore.</t>
+  </si>
+  <si>
+    <t>DSR-0350</t>
+  </si>
+  <si>
+    <t>Sheikh Telecom 2</t>
+  </si>
+  <si>
+    <t>Bonpara</t>
+  </si>
+  <si>
+    <t>Sheikh Saifuddin</t>
+  </si>
+  <si>
+    <t>Baraigram</t>
+  </si>
+  <si>
+    <t>Bonpara, Natore.</t>
+  </si>
+  <si>
+    <t>Azim Mobile Center</t>
+  </si>
+  <si>
+    <t>Md Azim Uddin</t>
+  </si>
+  <si>
+    <t>Koenbazar, Baraigram, Natore.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS Mobile </t>
+  </si>
+  <si>
+    <t>Md Rakib Ali</t>
+  </si>
+  <si>
+    <t>Gourango Hardware</t>
+  </si>
+  <si>
+    <t>Sree Gones Chandro</t>
+  </si>
+  <si>
+    <t>Shahebbazar, Baraigram, Natore.</t>
+  </si>
+  <si>
+    <t>Square  Telecom</t>
+  </si>
+  <si>
+    <t>Md Rony Ali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gopalpur, Lalpur, </t>
+  </si>
+  <si>
+    <t>Nirob Mobile &amp; Computer</t>
+  </si>
+  <si>
+    <t>Md Nirob Mahabur Rahman</t>
+  </si>
+  <si>
+    <t>Dayarampur, Bagatipara, Natore.</t>
   </si>
   <si>
     <t>Bagatipara</t>
-  </si>
-  <si>
-    <t>DSR-0619</t>
   </si>
 </sst>
 </file>
@@ -546,10 +576,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F20:F21"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -558,7 +588,7 @@
     <col min="2" max="2" width="9.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -644,16 +674,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -661,26 +691,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1712617115</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1303522382</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1303522382</v>
+        <v>1712617115</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -692,7 +722,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1303522382</v>
+        <v>1712617115</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
@@ -700,16 +730,16 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -717,26 +747,26 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1">
-        <v>1773666422</v>
+        <v>1714588737</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>1773666422</v>
+        <v>1714588737</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>22</v>
@@ -748,7 +778,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="1">
-        <v>1773666422</v>
+        <v>1714588737</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -756,16 +786,16 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
@@ -773,24 +803,26 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J4" s="1">
-        <v>1712459447</v>
+        <v>1712337781</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1">
-        <v>1712459447</v>
+        <v>1712337781</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>22</v>
@@ -802,112 +834,248 @@
         <v>21</v>
       </c>
       <c r="T4" s="1">
-        <v>1712459447</v>
+        <v>1712337781</v>
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1760264390</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="P5" s="1">
+        <v>1760264390</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1760264390</v>
+      </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1710372747</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="P6" s="1">
+        <v>1710372747</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1710372747</v>
+      </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="4"/>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1761689867</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="P7" s="1">
+        <v>1761689867</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1761689867</v>
+      </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="4"/>
+      <c r="I8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1791953259</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="P8" s="1">
+        <v>1791953259</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1791953259</v>
+      </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="4"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -915,9 +1083,31 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="6" t="s">
-        <v>37</v>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
31.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>RType</t>
   </si>
@@ -106,97 +106,85 @@
     <t>DSR-0350</t>
   </si>
   <si>
-    <t xml:space="preserve">ST Mobile </t>
-  </si>
-  <si>
-    <t>Gurudaspur</t>
-  </si>
-  <si>
-    <t>C.M Shoping Complex</t>
-  </si>
-  <si>
-    <t>Md Riad Talukdar</t>
-  </si>
-  <si>
-    <t>C.M Shoping Complex, Chaskoir</t>
-  </si>
-  <si>
     <t>DSR-0248</t>
   </si>
   <si>
-    <t>Mehedi Maruf Electronics</t>
-  </si>
-  <si>
-    <t>Md Masud Rana &amp; Touhid</t>
-  </si>
-  <si>
-    <t>Thana Road , Lalpur, Natore.</t>
-  </si>
-  <si>
-    <t>Abir Electronics</t>
-  </si>
-  <si>
     <t>Singra</t>
   </si>
   <si>
-    <t>Md Aslam Hossain</t>
-  </si>
-  <si>
-    <t>Kaligong Bazar, Singra, Natore</t>
-  </si>
-  <si>
     <t>DSR-0247</t>
   </si>
   <si>
-    <t>Ma Electronics</t>
-  </si>
-  <si>
-    <t>Nandangachi</t>
-  </si>
-  <si>
-    <t>Md Bodiuzzaman</t>
-  </si>
-  <si>
-    <t>1910362919-9</t>
-  </si>
-  <si>
-    <t>Rocket</t>
-  </si>
-  <si>
-    <t>Nandangachi, Puthia</t>
-  </si>
-  <si>
-    <t>Puthia</t>
-  </si>
-  <si>
     <t>Rajshahi</t>
   </si>
   <si>
-    <t>DSR-0351</t>
-  </si>
-  <si>
-    <t>Ma Mobile &amp; Sunglas Corner</t>
-  </si>
-  <si>
-    <t>Station Bazar</t>
-  </si>
-  <si>
-    <t>Sree Ashit Chakrobarti</t>
-  </si>
-  <si>
-    <t>Station Bazar, Natore.</t>
-  </si>
-  <si>
-    <t>Natore Sadar</t>
-  </si>
-  <si>
-    <t>Razib Mobile Zone</t>
-  </si>
-  <si>
-    <t>Md Razib Uddin</t>
-  </si>
-  <si>
-    <t>Tebaria, Natore</t>
+    <t>Arshi Electronics</t>
+  </si>
+  <si>
+    <t>Loxmicole</t>
+  </si>
+  <si>
+    <t>Md Abdullah Al Mamun</t>
+  </si>
+  <si>
+    <t>Baraigram</t>
+  </si>
+  <si>
+    <t>Laxmicole, Baraigram, Natore.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Telecom </t>
+  </si>
+  <si>
+    <t>Bagha</t>
+  </si>
+  <si>
+    <t>Md Babu Hosen</t>
+  </si>
+  <si>
+    <t>Arani Bazar, Bagha, Rajshahi.</t>
+  </si>
+  <si>
+    <t>Nabinogor Bohumukhi Somobai Somiti</t>
+  </si>
+  <si>
+    <t>Md Biplob Hossain</t>
+  </si>
+  <si>
+    <t>Nabinogor, Lalpur, Natore.</t>
+  </si>
+  <si>
+    <t>Nabil Computer</t>
+  </si>
+  <si>
+    <t>Kamruzzaman Pias</t>
+  </si>
+  <si>
+    <t>Bagha Bazar, Rajshahi.</t>
+  </si>
+  <si>
+    <t>Monia Telecom</t>
+  </si>
+  <si>
+    <t>Jonail</t>
+  </si>
+  <si>
+    <t>Jonail Bazar, Baraigram, Natore.</t>
+  </si>
+  <si>
+    <t>Md Munjur Alam</t>
+  </si>
+  <si>
+    <t>Alamin Telecom</t>
+  </si>
+  <si>
+    <t>Md Khorshed Vandary</t>
+  </si>
+  <si>
+    <t>Sigra.</t>
+  </si>
+  <si>
+    <t>DSR-0349</t>
   </si>
 </sst>
 </file>
@@ -600,14 +588,14 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="6" bestFit="1" customWidth="1"/>
@@ -695,16 +683,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -712,26 +700,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1">
-        <v>1780944636</v>
+        <v>1726359224</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1780944636</v>
+        <v>1726359224</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -743,7 +731,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1780944636</v>
+        <v>1726359224</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
@@ -751,16 +739,16 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -768,26 +756,26 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J3" s="1">
-        <v>1748934030</v>
+        <v>1740418484</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>1748934030</v>
+        <v>1740418484</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>22</v>
@@ -799,7 +787,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="1">
-        <v>1748934030</v>
+        <v>1740418484</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -807,16 +795,16 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
@@ -824,26 +812,26 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J4" s="1">
-        <v>1719928921</v>
+        <v>1839178501</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1">
-        <v>1719928921</v>
+        <v>1839178501</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>22</v>
@@ -855,7 +843,7 @@
         <v>21</v>
       </c>
       <c r="T4" s="1">
-        <v>1719928921</v>
+        <v>1839178501</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -863,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
@@ -880,26 +868,26 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J5" s="1">
-        <v>1910362919</v>
+        <v>1710002659</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1">
-        <v>1910362919</v>
+        <v>1710002659</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>22</v>
@@ -908,10 +896,10 @@
         <v>25</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1710002659</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -919,16 +907,16 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -936,26 +924,26 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1">
-        <v>1787227734</v>
+        <v>1770800299</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1">
-        <v>1787227734</v>
+        <v>1770800299</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>22</v>
@@ -967,7 +955,7 @@
         <v>21</v>
       </c>
       <c r="T6" s="1">
-        <v>1787227734</v>
+        <v>1770800299</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -975,16 +963,16 @@
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -992,26 +980,26 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J7" s="1">
-        <v>1713342035</v>
+        <v>1762676884</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1">
-        <v>1713342035</v>
+        <v>1762676884</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>22</v>
@@ -1023,7 +1011,7 @@
         <v>21</v>
       </c>
       <c r="T7" s="1">
-        <v>1713342035</v>
+        <v>1762676884</v>
       </c>
     </row>
     <row r="8" spans="1:20">

</xml_diff>

<commit_message>
04.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>RType</t>
   </si>
@@ -106,9 +106,6 @@
     <t>DSR-0350</t>
   </si>
   <si>
-    <t>DSR-0248</t>
-  </si>
-  <si>
     <t>Singra</t>
   </si>
   <si>
@@ -118,73 +115,91 @@
     <t>Rajshahi</t>
   </si>
   <si>
-    <t>Arshi Electronics</t>
-  </si>
-  <si>
-    <t>Loxmicole</t>
-  </si>
-  <si>
-    <t>Md Abdullah Al Mamun</t>
-  </si>
-  <si>
-    <t>Baraigram</t>
-  </si>
-  <si>
-    <t>Laxmicole, Baraigram, Natore.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ma Telecom </t>
-  </si>
-  <si>
     <t>Bagha</t>
   </si>
   <si>
-    <t>Md Babu Hosen</t>
-  </si>
-  <si>
     <t>Arani Bazar, Bagha, Rajshahi.</t>
   </si>
   <si>
-    <t>Nabinogor Bohumukhi Somobai Somiti</t>
-  </si>
-  <si>
-    <t>Md Biplob Hossain</t>
-  </si>
-  <si>
-    <t>Nabinogor, Lalpur, Natore.</t>
-  </si>
-  <si>
-    <t>Nabil Computer</t>
-  </si>
-  <si>
-    <t>Kamruzzaman Pias</t>
-  </si>
-  <si>
-    <t>Bagha Bazar, Rajshahi.</t>
-  </si>
-  <si>
-    <t>Monia Telecom</t>
-  </si>
-  <si>
-    <t>Jonail</t>
-  </si>
-  <si>
-    <t>Jonail Bazar, Baraigram, Natore.</t>
-  </si>
-  <si>
-    <t>Md Munjur Alam</t>
-  </si>
-  <si>
-    <t>Alamin Telecom</t>
-  </si>
-  <si>
-    <t>Md Khorshed Vandary</t>
-  </si>
-  <si>
-    <t>Sigra.</t>
-  </si>
-  <si>
     <t>DSR-0349</t>
+  </si>
+  <si>
+    <t>Saikot Telecom</t>
+  </si>
+  <si>
+    <t>Jholmolia</t>
+  </si>
+  <si>
+    <t>Md Saikot Islam</t>
+  </si>
+  <si>
+    <t>Jholmolia Bazar, Puthia, Rajshahi.</t>
+  </si>
+  <si>
+    <t>Puthia</t>
+  </si>
+  <si>
+    <t>Bismillah Mobile Shop 2</t>
+  </si>
+  <si>
+    <t>Md Hasan Ali</t>
+  </si>
+  <si>
+    <t>Liton Electronics &amp; Sound System</t>
+  </si>
+  <si>
+    <t>Abdulpur</t>
+  </si>
+  <si>
+    <t>Arani</t>
+  </si>
+  <si>
+    <t>Md Shoriful Islam Liton</t>
+  </si>
+  <si>
+    <t>Abdulpur, Lalpur, Natore.</t>
+  </si>
+  <si>
+    <t>DSR-0351</t>
+  </si>
+  <si>
+    <t>Motin Traders</t>
+  </si>
+  <si>
+    <t>Kafuria</t>
+  </si>
+  <si>
+    <t>Md Motin Ali</t>
+  </si>
+  <si>
+    <t>Kafuria,Natore Sadar, Natore.</t>
+  </si>
+  <si>
+    <t>Natore Sadar</t>
+  </si>
+  <si>
+    <t>GD Electronics</t>
+  </si>
+  <si>
+    <t>Serkul</t>
+  </si>
+  <si>
+    <t>Md Masud Rana</t>
+  </si>
+  <si>
+    <t>Serkul,Sigra.</t>
+  </si>
+  <si>
+    <t>Apu Topu Electronics</t>
+  </si>
+  <si>
+    <t>Station Bazar</t>
+  </si>
+  <si>
+    <t>Sree Tapos Chakrobortti</t>
+  </si>
+  <si>
+    <t>Station Bazar, Natore.</t>
   </si>
 </sst>
 </file>
@@ -585,10 +600,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,16 +698,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -700,26 +715,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1">
-        <v>1726359224</v>
+        <v>1906270807</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1726359224</v>
+        <v>1906270807</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -731,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1726359224</v>
+        <v>1906270807</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
@@ -739,16 +754,16 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -756,26 +771,26 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J3" s="1">
-        <v>1740418484</v>
+        <v>1754557390</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>1740418484</v>
+        <v>1754557390</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>22</v>
@@ -787,7 +802,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="1">
-        <v>1740418484</v>
+        <v>1754557390</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -801,10 +816,10 @@
         <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
@@ -812,10 +827,10 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J4" s="1">
-        <v>1839178501</v>
+        <v>1740821951</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>24</v>
@@ -827,11 +842,11 @@
         <v>26</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1">
-        <v>1839178501</v>
+        <v>1740821951</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>22</v>
@@ -843,7 +858,7 @@
         <v>21</v>
       </c>
       <c r="T4" s="1">
-        <v>1839178501</v>
+        <v>1740821951</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -851,16 +866,16 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
@@ -868,26 +883,26 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J5" s="1">
-        <v>1710002659</v>
+        <v>1745743895</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1">
-        <v>1710002659</v>
+        <v>1745743895</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>22</v>
@@ -899,7 +914,7 @@
         <v>21</v>
       </c>
       <c r="T5" s="1">
-        <v>1710002659</v>
+        <v>1745743895</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -907,16 +922,16 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -924,26 +939,26 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J6" s="1">
-        <v>1770800299</v>
+        <v>1755068758</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1">
-        <v>1770800299</v>
+        <v>1755068758</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>22</v>
@@ -955,7 +970,7 @@
         <v>21</v>
       </c>
       <c r="T6" s="1">
-        <v>1770800299</v>
+        <v>1755068758</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -963,16 +978,16 @@
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -980,26 +995,26 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J7" s="1">
-        <v>1762676884</v>
+        <v>1730902795</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1">
-        <v>1762676884</v>
+        <v>1730902795</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>22</v>
@@ -1011,24 +1026,24 @@
         <v>21</v>
       </c>
       <c r="T7" s="1">
-        <v>1762676884</v>
+        <v>1730902795</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="4"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1040,17 +1055,17 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="4"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1058,30 +1073,8 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="6" t="s">
+    <row r="20" spans="5:5">
+      <c r="E20" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19.11.2020 MC SAles Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>RType</t>
   </si>
@@ -94,46 +94,28 @@
     <t>Rural</t>
   </si>
   <si>
-    <t>ZSO-0022</t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>Natore Sadar</t>
-  </si>
-  <si>
-    <t>Dubai Mobile Center</t>
-  </si>
-  <si>
-    <t>Central Mosjid Market</t>
-  </si>
-  <si>
-    <t>Md Rafiqul Islam Sikder</t>
-  </si>
-  <si>
-    <t>Central Masjid Market, Natore</t>
-  </si>
-  <si>
-    <t>DSR-0246</t>
-  </si>
-  <si>
-    <t>Masum Electric &amp; Electronics</t>
-  </si>
-  <si>
-    <t>Moukhura</t>
-  </si>
-  <si>
-    <t>Md Yakub Ali Master</t>
-  </si>
-  <si>
-    <t>Moukhura, Baraigram, Natore.</t>
-  </si>
-  <si>
-    <t>Baraigram</t>
-  </si>
-  <si>
-    <t>DSR-0248</t>
+    <t>Laxmi Telecom</t>
+  </si>
+  <si>
+    <t>Chatni Bazar</t>
+  </si>
+  <si>
+    <t>Bokul Mondol</t>
+  </si>
+  <si>
+    <t>Naldanga</t>
+  </si>
+  <si>
+    <t>ZSO-0025</t>
+  </si>
+  <si>
+    <t>Chatni, Shibpur, Naldanga</t>
+  </si>
+  <si>
+    <t>DSR-0247</t>
   </si>
 </sst>
 </file>
@@ -537,7 +519,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F22" sqref="F21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,13 +617,13 @@
         <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -649,26 +631,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1">
-        <v>1740976030</v>
+        <v>1736044956</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1740976030</v>
+        <v>1736044956</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -680,64 +662,30 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1733260871</v>
+        <v>1736044956</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1717670951</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1">
-        <v>1717670951</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="1">
-        <v>1717670951</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1"/>
@@ -873,7 +821,7 @@
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
30.11.2020 MC Capital Statement
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -97,18 +97,6 @@
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>DSR-0247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayer Doa </t>
-  </si>
-  <si>
-    <t>Valugachi</t>
-  </si>
-  <si>
-    <t>Ruhul Amin</t>
-  </si>
-  <si>
     <t>DSR-0351</t>
   </si>
   <si>
@@ -118,25 +106,37 @@
     <t>Rajshahi</t>
   </si>
   <si>
-    <t>Valugachi, Naopara,Puthia, Rajshahi</t>
-  </si>
-  <si>
-    <t>Babu Electronics</t>
-  </si>
-  <si>
-    <t>Islabari</t>
-  </si>
-  <si>
-    <t>Md Babu Hosen</t>
-  </si>
-  <si>
-    <t>Natore Sadar</t>
-  </si>
-  <si>
     <t>ZSO-0023</t>
   </si>
   <si>
-    <t>Islabari, Natore</t>
+    <t>Masum Electronics</t>
+  </si>
+  <si>
+    <t>Khidilpur</t>
+  </si>
+  <si>
+    <t>Md Masum Ali</t>
+  </si>
+  <si>
+    <t>Baraigram</t>
+  </si>
+  <si>
+    <t>Khidilpur Bazar, Mokhura,Baraigram</t>
+  </si>
+  <si>
+    <t>DSR-0248</t>
+  </si>
+  <si>
+    <t>SR Telecom</t>
+  </si>
+  <si>
+    <t>Jholmolia</t>
+  </si>
+  <si>
+    <t>Maqsudur Rahman</t>
+  </si>
+  <si>
+    <t>Jholmolia , Puthia, Rajshahi</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,16 +635,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -652,26 +652,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1632005795</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1">
-        <v>1827156464</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1827156464</v>
+        <v>1632005795</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -683,7 +683,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1827156464</v>
+        <v>1632005795</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
@@ -694,13 +694,13 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -708,26 +708,26 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1">
-        <v>1723632345</v>
+        <v>1768927219</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>1723632345</v>
+        <v>1768927219</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>22</v>
@@ -739,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="1">
-        <v>1723632345</v>
+        <v>1768927219</v>
       </c>
     </row>
     <row r="4" spans="1:20">

</xml_diff>

<commit_message>
17.12.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>RType</t>
   </si>
@@ -109,27 +109,12 @@
     <t>ZSO-0023</t>
   </si>
   <si>
-    <t>Masum Electronics</t>
-  </si>
-  <si>
-    <t>Khidilpur</t>
-  </si>
-  <si>
-    <t>Md Masum Ali</t>
-  </si>
-  <si>
     <t>Baraigram</t>
   </si>
   <si>
-    <t>Khidilpur Bazar, Mokhura,Baraigram</t>
-  </si>
-  <si>
     <t>DSR-0248</t>
   </si>
   <si>
-    <t>SR Telecom</t>
-  </si>
-  <si>
     <t>Jholmolia</t>
   </si>
   <si>
@@ -137,6 +122,18 @@
   </si>
   <si>
     <t>Jholmolia , Puthia, Rajshahi</t>
+  </si>
+  <si>
+    <t>Achol Telecom</t>
+  </si>
+  <si>
+    <t>Jonail</t>
+  </si>
+  <si>
+    <t>Arifur Rahman</t>
+  </si>
+  <si>
+    <t>Jonail, Baraigram,Natore.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +537,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,16 +632,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -652,26 +649,26 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1">
-        <v>1632005795</v>
+        <v>1912021212</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <v>1632005795</v>
+        <v>1912021212</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
@@ -683,7 +680,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="1">
-        <v>1632005795</v>
+        <v>1912021212</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="5" customFormat="1">
@@ -693,14 +690,12 @@
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -708,7 +703,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1">
         <v>1768927219</v>
@@ -723,7 +718,7 @@
         <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">

</xml_diff>

<commit_message>
21.12.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
+++ b/2020/Others/Adding New Retailer Format/Adding new retailers format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>RType</t>
   </si>
@@ -97,33 +97,12 @@
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>DSR-0351</t>
-  </si>
-  <si>
-    <t>Puthia</t>
-  </si>
-  <si>
-    <t>Rajshahi</t>
-  </si>
-  <si>
-    <t>ZSO-0023</t>
-  </si>
-  <si>
     <t>Baraigram</t>
   </si>
   <si>
     <t>DSR-0248</t>
   </si>
   <si>
-    <t>Jholmolia</t>
-  </si>
-  <si>
-    <t>Maqsudur Rahman</t>
-  </si>
-  <si>
-    <t>Jholmolia , Puthia, Rajshahi</t>
-  </si>
-  <si>
     <t>Achol Telecom</t>
   </si>
   <si>
@@ -134,6 +113,24 @@
   </si>
   <si>
     <t>Jonail, Baraigram,Natore.</t>
+  </si>
+  <si>
+    <t>Mayer Doa Varaitey Store</t>
+  </si>
+  <si>
+    <t>Lalpur</t>
+  </si>
+  <si>
+    <t>Md Abu Salek</t>
+  </si>
+  <si>
+    <t>Chinir Bottola, Lalpur, Natore</t>
+  </si>
+  <si>
+    <t>DSR-0350</t>
+  </si>
+  <si>
+    <t>ZSO-0025</t>
   </si>
 </sst>
 </file>
@@ -537,7 +534,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,16 +629,16 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -649,7 +646,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1">
         <v>1912021212</v>
@@ -658,13 +655,13 @@
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
@@ -688,14 +685,16 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -703,26 +702,26 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J3" s="1">
         <v>1768927219</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>1768927219</v>
+        <v>1738027070</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>22</v>
@@ -734,7 +733,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="1">
-        <v>1768927219</v>
+        <v>1738027070</v>
       </c>
     </row>
     <row r="4" spans="1:20">

</xml_diff>